<commit_message>
Ajout de fonction dans gestion_BDD_materiaux.py pour afficher les materiaux
Modification de main pour ne demander qu'une fois les conditions initiales et ajout de la phase de calcul

Ajout de fonctions de tracé de pression et vitesse dans gestion_traces.py
</commit_message>
<xml_diff>
--- a/BDD_materiaux.xlsx
+++ b/BDD_materiaux.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amark\PycharmProjects\PipeHelper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5CBA1C06-8A24-4EA0-9D66-080C7A70CA08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD88B0DE-7B3E-438C-837B-79031DA9A7A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="230" yWindow="1170" windowWidth="14400" windowHeight="8170" xr2:uid="{EA5947BA-C433-4438-B3A0-8CEF39250B97}"/>
+    <workbookView xWindow="340" yWindow="1170" windowWidth="14400" windowHeight="8170" xr2:uid="{EA5947BA-C433-4438-B3A0-8CEF39250B97}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>Rugosité</t>
   </si>
   <si>
-    <t>Conduites étirées</t>
-  </si>
-  <si>
     <t>Conduites en PVC et polyéthylène</t>
   </si>
   <si>
@@ -85,6 +82,9 @@
   </si>
   <si>
     <t>Conduits maçonnés</t>
+  </si>
+  <si>
+    <t>Conduites étirées : aluminium, cuivre, …</t>
   </si>
 </sst>
 </file>
@@ -439,10 +439,13 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B13"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="42.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -454,7 +457,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>1.5E-3</v>
@@ -462,7 +465,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>7.0000000000000001E-3</v>
@@ -470,7 +473,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>4.4999999999999998E-2</v>
@@ -478,7 +481,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>7.4999999999999997E-2</v>
@@ -486,7 +489,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>0.125</v>
@@ -494,7 +497,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>0.15</v>
@@ -502,7 +505,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>0.15</v>
@@ -510,7 +513,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>0.6</v>
@@ -518,7 +521,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>0.6</v>
@@ -526,7 +529,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>0.5</v>
@@ -534,7 +537,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>1.3</v>
@@ -542,7 +545,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>1.5</v>
@@ -550,7 +553,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -558,7 +561,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -566,7 +569,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>4</v>

</xml_diff>

<commit_message>
Ajout d'une fonction test de perte de charge regu
</commit_message>
<xml_diff>
--- a/BDD_materiaux.xlsx
+++ b/BDD_materiaux.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amark\PycharmProjects\PipeHelper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD88B0DE-7B3E-438C-837B-79031DA9A7A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58DABB3-95A5-4E24-9212-214A9CD4B112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="1170" windowWidth="14400" windowHeight="8170" xr2:uid="{EA5947BA-C433-4438-B3A0-8CEF39250B97}"/>
+    <workbookView xWindow="4910" yWindow="110" windowWidth="14400" windowHeight="8170" xr2:uid="{EA5947BA-C433-4438-B3A0-8CEF39250B97}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Matériaux</t>
   </si>
@@ -42,49 +42,55 @@
     <t>Rugosité</t>
   </si>
   <si>
-    <t>Conduites en PVC et polyéthylène</t>
-  </si>
-  <si>
-    <t>Tuyauterie en acier du commmerce</t>
-  </si>
-  <si>
-    <t>Conduites en amiante-ciment</t>
-  </si>
-  <si>
-    <t>Tuyauteries en fonte asphaltées</t>
-  </si>
-  <si>
-    <t>Conduits en tçole d'acier agrafés</t>
-  </si>
-  <si>
-    <t>Tuyauteries en acier galvanisé</t>
-  </si>
-  <si>
-    <t>Tuyauteries en acier rouillées</t>
-  </si>
-  <si>
-    <t>Conduits en bois</t>
-  </si>
-  <si>
-    <t>Tuyauteries en fonte</t>
-  </si>
-  <si>
-    <t>Conduits souples agrafés en spirale</t>
-  </si>
-  <si>
-    <t>Conduits treillis métallique et enduit</t>
-  </si>
-  <si>
-    <t>Tuyauteries en acier très rouillées</t>
-  </si>
-  <si>
-    <t>Conduits en béton brut de décoffrage</t>
-  </si>
-  <si>
-    <t>Conduits maçonnés</t>
-  </si>
-  <si>
-    <t>Conduites étirées : aluminium, cuivre, …</t>
+    <t>cuivre, plomb, laiton, inox</t>
+  </si>
+  <si>
+    <t>PVC</t>
+  </si>
+  <si>
+    <t>acier inox</t>
+  </si>
+  <si>
+    <t>tube acier du commerce</t>
+  </si>
+  <si>
+    <t>acier étiré</t>
+  </si>
+  <si>
+    <t>acier soudé</t>
+  </si>
+  <si>
+    <t>acier galvanisé</t>
+  </si>
+  <si>
+    <t>acier rouillé</t>
+  </si>
+  <si>
+    <t>fonte usagée</t>
+  </si>
+  <si>
+    <t>fonte neuve</t>
+  </si>
+  <si>
+    <t>fonte incrustée</t>
+  </si>
+  <si>
+    <t>tôle ou fonte asphaltée</t>
+  </si>
+  <si>
+    <t>ciment bien lissé</t>
+  </si>
+  <si>
+    <t>béton ordinaire</t>
+  </si>
+  <si>
+    <t>béton grossier</t>
+  </si>
+  <si>
+    <t>bois bien raboté</t>
+  </si>
+  <si>
+    <t>bois ordinaire</t>
   </si>
 </sst>
 </file>
@@ -120,8 +126,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A70E646B-A065-4AEF-B605-A09C22EABE56}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -457,55 +464,55 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>1.5E-3</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>7.0000000000000001E-3</v>
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1.5E-3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>4.4999999999999998E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>7.4999999999999997E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>0.125</v>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>0.15</v>
+        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>0.15</v>
@@ -513,18 +520,18 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9">
-        <v>0.6</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -532,47 +539,63 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0.5</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12">
-        <v>1.3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13">
-        <v>1.5</v>
+        <v>1.2E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dernières modifications avant présentation
</commit_message>
<xml_diff>
--- a/BDD_materiaux.xlsx
+++ b/BDD_materiaux.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amark\PycharmProjects\PipeHelper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58DABB3-95A5-4E24-9212-214A9CD4B112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3974BD6E-2855-4AE1-9C70-64BB94010084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4910" yWindow="110" windowWidth="14400" windowHeight="8170" xr2:uid="{EA5947BA-C433-4438-B3A0-8CEF39250B97}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Matériaux</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>bois ordinaire</t>
+  </si>
+  <si>
+    <t>aluminium</t>
+  </si>
+  <si>
+    <t>Polyéthylène</t>
   </si>
 </sst>
 </file>
@@ -443,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A70E646B-A065-4AEF-B605-A09C22EABE56}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -598,6 +604,22 @@
         <v>1</v>
       </c>
     </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>2E-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>